<commit_message>
Add parsed json functionality
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -564,7 +564,7 @@
         <v>ACEITUNA CASTELL BALDE 5 Kgs</v>
       </c>
       <c r="C15" t="str">
-        <v/>
+        <v>42010</v>
       </c>
     </row>
     <row r="16">
@@ -575,7 +575,7 @@
         <v>ACEITUNA CASTELL RODAJA 70 Grs</v>
       </c>
       <c r="C16" t="str">
-        <v/>
+        <v>40195</v>
       </c>
     </row>
     <row r="17">
@@ -586,7 +586,7 @@
         <v>ACEITUNA CASTELL S/CAROZO 150 Grs</v>
       </c>
       <c r="C17" t="str">
-        <v/>
+        <v>40187</v>
       </c>
     </row>
     <row r="18">
@@ -597,7 +597,7 @@
         <v>ACEITUNA CEBILA 100 Grs</v>
       </c>
       <c r="C18" t="str">
-        <v/>
+        <v>41452</v>
       </c>
     </row>
     <row r="19">
@@ -608,7 +608,7 @@
         <v>ACELGA LA BANDA LATA 800 Grs</v>
       </c>
       <c r="C19" t="str">
-        <v/>
+        <v>42000</v>
       </c>
     </row>
     <row r="20">
@@ -784,7 +784,7 @@
         <v>ALCOHOL ET. ALCOPROTEC 96% 1 Lt.</v>
       </c>
       <c r="C35" t="str">
-        <v/>
+        <v>41497</v>
       </c>
     </row>
     <row r="36">
@@ -795,7 +795,7 @@
         <v>ALCOHOL ET. ALCOPROTEC 96% 500 CC.</v>
       </c>
       <c r="C36" t="str">
-        <v/>
+        <v>41496</v>
       </c>
     </row>
     <row r="37">
@@ -806,7 +806,7 @@
         <v>ALCOHOL ET. BIALCOHOL 70% 1 Lt.</v>
       </c>
       <c r="C37" t="str">
-        <v/>
+        <v>40018</v>
       </c>
     </row>
     <row r="38">
@@ -817,7 +817,7 @@
         <v>ALCOHOL ET. BIALCOHOL 70% 500 CC.</v>
       </c>
       <c r="C38" t="str">
-        <v/>
+        <v>40019</v>
       </c>
     </row>
     <row r="39">
@@ -828,7 +828,7 @@
         <v>ALCOHOL ET. BIALCOHOL 96% 1 Lt.</v>
       </c>
       <c r="C39" t="str">
-        <v/>
+        <v>40383</v>
       </c>
     </row>
     <row r="40">
@@ -839,7 +839,7 @@
         <v>ALCOHOL ET. BIALCOHOL 96% 500 CC.</v>
       </c>
       <c r="C40" t="str">
-        <v/>
+        <v>41276</v>
       </c>
     </row>
     <row r="41">
@@ -850,7 +850,7 @@
         <v>ALCOHOL QUEMAR BIALCOHOL 1 Lt.</v>
       </c>
       <c r="C41" t="str">
-        <v/>
+        <v>40996</v>
       </c>
     </row>
     <row r="42">
@@ -861,7 +861,7 @@
         <v>ALCOHOL QUEMAR BIALCOHOL 500 ml.</v>
       </c>
       <c r="C42" t="str">
-        <v/>
+        <v>41387</v>
       </c>
     </row>
     <row r="43">
@@ -872,7 +872,7 @@
         <v>ALGODON ESTRELLA CLASICO 75 Grs</v>
       </c>
       <c r="C43" t="str">
-        <v/>
+        <v>30428</v>
       </c>
     </row>
     <row r="44">
@@ -1367,7 +1367,7 @@
         <v>ARROZ GALLO CARNAROLI 5 Kgs</v>
       </c>
       <c r="C88" t="str">
-        <v/>
+        <v>30353</v>
       </c>
     </row>
     <row r="89">
@@ -1378,7 +1378,7 @@
         <v>ARROZ GALLO ORO 1 Kgs</v>
       </c>
       <c r="C89" t="str">
-        <v/>
+        <v>30340</v>
       </c>
     </row>
     <row r="90">
@@ -1389,7 +1389,7 @@
         <v>ARROZ GALLO ORO 500 Grs</v>
       </c>
       <c r="C90" t="str">
-        <v/>
+        <v>30338</v>
       </c>
     </row>
     <row r="91">
@@ -1400,7 +1400,7 @@
         <v>ARROZ GALLO ORO Bolsa 1 Kgs</v>
       </c>
       <c r="C91" t="str">
-        <v/>
+        <v>30336</v>
       </c>
     </row>
     <row r="92">
@@ -1477,7 +1477,7 @@
         <v>ARVEJA LA BANDA LATA 800 Grs</v>
       </c>
       <c r="C98" t="str">
-        <v/>
+        <v>42001</v>
       </c>
     </row>
     <row r="99">
@@ -1488,7 +1488,7 @@
         <v>ARVEJA MAROLIO TETRA 340 Grs</v>
       </c>
       <c r="C99" t="str">
-        <v/>
+        <v>41000</v>
       </c>
     </row>
     <row r="100">
@@ -1675,7 +1675,7 @@
         <v>AZUCAR AZUCEL 1 Kgs</v>
       </c>
       <c r="C116" t="str">
-        <v/>
+        <v>40074</v>
       </c>
     </row>
     <row r="117">
@@ -1686,7 +1686,7 @@
         <v>AZUCAR LEDESMA 1 Kgs</v>
       </c>
       <c r="C117" t="str">
-        <v/>
+        <v>40879</v>
       </c>
     </row>
     <row r="118">
@@ -1697,7 +1697,7 @@
         <v>AZUCAR LEDESMA LIGHT 500 Grs</v>
       </c>
       <c r="C118" t="str">
-        <v/>
+        <v>40909</v>
       </c>
     </row>
     <row r="119">
@@ -1708,7 +1708,7 @@
         <v>AZUCAR LEDESMA RUBIA 900 Un.</v>
       </c>
       <c r="C119" t="str">
-        <v/>
+        <v>41499</v>
       </c>
     </row>
     <row r="120">
@@ -1719,7 +1719,7 @@
         <v>AZUCAR LEDESMA SOBRES 1000 Un.</v>
       </c>
       <c r="C120" t="str">
-        <v/>
+        <v>41197</v>
       </c>
     </row>
     <row r="121">
@@ -1752,7 +1752,7 @@
         <v>BIZC. RAVANA CHOCOLATE 540 Grs</v>
       </c>
       <c r="C123" t="str">
-        <v/>
+        <v>40564</v>
       </c>
     </row>
     <row r="124">
@@ -1763,7 +1763,7 @@
         <v>BIZCOCHOS DON SATUR DULCES 200 Grs</v>
       </c>
       <c r="C124" t="str">
-        <v/>
+        <v>40084</v>
       </c>
     </row>
     <row r="125">
@@ -1774,7 +1774,7 @@
         <v>BIZCOCHOS DON SATUR SALADOS 200 Grs</v>
       </c>
       <c r="C125" t="str">
-        <v/>
+        <v>40083</v>
       </c>
     </row>
     <row r="126">
@@ -1785,7 +1785,7 @@
         <v>BOCADITOS GRANIX RELLENO FRUTILLA 180 Grs</v>
       </c>
       <c r="C126" t="str">
-        <v/>
+        <v>41435</v>
       </c>
     </row>
     <row r="127">
@@ -1829,7 +1829,7 @@
         <v>CAFE ARLISTAN 100 Grs</v>
       </c>
       <c r="C130" t="str">
-        <v/>
+        <v>30024</v>
       </c>
     </row>
     <row r="131">
@@ -1840,7 +1840,7 @@
         <v>CAFE ARLISTAN 170 Grs</v>
       </c>
       <c r="C131" t="str">
-        <v/>
+        <v>30022</v>
       </c>
     </row>
     <row r="132">
@@ -1851,7 +1851,7 @@
         <v>CAFE CRYSF Saquitos 20 Un.</v>
       </c>
       <c r="C132" t="str">
-        <v/>
+        <v>30071</v>
       </c>
     </row>
     <row r="133">
@@ -1884,7 +1884,7 @@
         <v>CAFE PLANTA DE CAFE MOLIDO 125 Grs</v>
       </c>
       <c r="C135" t="str">
-        <v/>
+        <v>40013</v>
       </c>
     </row>
     <row r="136">
@@ -2159,7 +2159,7 @@
         <v>CHAMPIGNON CARACAS ENTERO 400 Grs</v>
       </c>
       <c r="C160" t="str">
-        <v/>
+        <v>40129</v>
       </c>
     </row>
     <row r="161">
@@ -2170,7 +2170,7 @@
         <v>CHOCLO GR.AMAR BONDUELLE LATA 225 Grs</v>
       </c>
       <c r="C161" t="str">
-        <v/>
+        <v>40135</v>
       </c>
     </row>
     <row r="162">
@@ -2181,7 +2181,7 @@
         <v>CHOCLO GR.AMAR LA BANDA LATA 810 Grs</v>
       </c>
       <c r="C162" t="str">
-        <v/>
+        <v>42003</v>
       </c>
     </row>
     <row r="163">
@@ -2192,7 +2192,7 @@
         <v>CHOCLO GR.AMAR MAROLIO LATA 300 Grs</v>
       </c>
       <c r="C163" t="str">
-        <v/>
+        <v>41009</v>
       </c>
     </row>
     <row r="164">
@@ -2621,7 +2621,7 @@
         <v>DISCOS DONCELLA ALGODON 80 Un.</v>
       </c>
       <c r="C202" t="str">
-        <v/>
+        <v>50430</v>
       </c>
     </row>
     <row r="203">
@@ -2731,7 +2731,7 @@
         <v>EDULCORANTE CA�UELAS Clasico 100 Un.</v>
       </c>
       <c r="C212" t="str">
-        <v/>
+        <v>41492</v>
       </c>
     </row>
     <row r="213">
@@ -2753,7 +2753,7 @@
         <v>EDULCORANTE HILERET Clasico 100 Un.</v>
       </c>
       <c r="C214" t="str">
-        <v/>
+        <v>40249</v>
       </c>
     </row>
     <row r="215">
@@ -2764,7 +2764,7 @@
         <v>EDULCORANTE HILERET Clasico 50 Un.</v>
       </c>
       <c r="C215" t="str">
-        <v/>
+        <v>40248</v>
       </c>
     </row>
     <row r="216">
@@ -2775,7 +2775,7 @@
         <v>EDULCORANTE HILERET Clasico 500 Un.</v>
       </c>
       <c r="C216" t="str">
-        <v/>
+        <v>40406</v>
       </c>
     </row>
     <row r="217">
@@ -2786,7 +2786,7 @@
         <v>EDULCORANTE HILERET Clasico LIQ 250 CC.</v>
       </c>
       <c r="C217" t="str">
-        <v/>
+        <v>40250</v>
       </c>
     </row>
     <row r="218">
@@ -2797,7 +2797,7 @@
         <v>EDULCORANTE HILERET Clasico LIQ 500 CC.</v>
       </c>
       <c r="C218" t="str">
-        <v/>
+        <v>40251</v>
       </c>
     </row>
     <row r="219">
@@ -2808,7 +2808,7 @@
         <v>EDULCORANTE HILERET Mate LIQ 200 CC.</v>
       </c>
       <c r="C219" t="str">
-        <v/>
+        <v>40262</v>
       </c>
     </row>
     <row r="220">
@@ -2819,7 +2819,7 @@
         <v>EDULCORANTE HILERET Stevia 100 Un.</v>
       </c>
       <c r="C220" t="str">
-        <v/>
+        <v>40253</v>
       </c>
     </row>
     <row r="221">
@@ -2830,7 +2830,7 @@
         <v>EDULCORANTE HILERET Sweet 50 Un.</v>
       </c>
       <c r="C221" t="str">
-        <v/>
+        <v>40255</v>
       </c>
     </row>
     <row r="222">
@@ -2841,7 +2841,7 @@
         <v>EDULCORANTE HILERET Zucra 50 Un.</v>
       </c>
       <c r="C222" t="str">
-        <v/>
+        <v>40259</v>
       </c>
     </row>
     <row r="223">
@@ -2852,7 +2852,7 @@
         <v>EDULCORANTE HILERET Zucra LIQ 200 CC.</v>
       </c>
       <c r="C223" t="str">
-        <v/>
+        <v>40261</v>
       </c>
     </row>
     <row r="224">
@@ -2863,7 +2863,7 @@
         <v>EDULCORANTE LEDESMA STEVIA 200 Un.</v>
       </c>
       <c r="C224" t="str">
-        <v/>
+        <v>40503</v>
       </c>
     </row>
     <row r="225">
@@ -2874,7 +2874,7 @@
         <v>ENCENDEDOR CANDELA Un.</v>
       </c>
       <c r="C225" t="str">
-        <v/>
+        <v>41915</v>
       </c>
     </row>
     <row r="226">
@@ -2885,7 +2885,7 @@
         <v>ESPINACA LA BANDA LATA 800 Grs</v>
       </c>
       <c r="C226" t="str">
-        <v/>
+        <v>42002</v>
       </c>
     </row>
     <row r="227">
@@ -2940,7 +2940,7 @@
         <v>FID. DON BERNABEU CODITO 500 Grs</v>
       </c>
       <c r="C231" t="str">
-        <v/>
+        <v>41273</v>
       </c>
     </row>
     <row r="232">
@@ -2951,7 +2951,7 @@
         <v>FID. DON BERNABEU MOSTACHOL 500 Grs</v>
       </c>
       <c r="C232" t="str">
-        <v/>
+        <v>41271</v>
       </c>
     </row>
     <row r="233">
@@ -2962,7 +2962,7 @@
         <v>FID. DON BERNABEU RIGATTI 500 Grs</v>
       </c>
       <c r="C233" t="str">
-        <v/>
+        <v>41272</v>
       </c>
     </row>
     <row r="234">
@@ -2973,7 +2973,7 @@
         <v>FID. DON BERNABEU SPAGHETTI 500 Grs</v>
       </c>
       <c r="C234" t="str">
-        <v/>
+        <v>41268</v>
       </c>
     </row>
     <row r="235">
@@ -2984,7 +2984,7 @@
         <v>FID. DON BERNABEU TALLARIN 500 Grs</v>
       </c>
       <c r="C235" t="str">
-        <v/>
+        <v>41269</v>
       </c>
     </row>
     <row r="236">
@@ -2995,7 +2995,7 @@
         <v>FID. DON BERNABEU TIRABUZON 500 Grs</v>
       </c>
       <c r="C236" t="str">
-        <v/>
+        <v>41270</v>
       </c>
     </row>
     <row r="237">
@@ -3116,7 +3116,7 @@
         <v>FID. MAROLIO CAB.ANGEL 500 Grs</v>
       </c>
       <c r="C247" t="str">
-        <v/>
+        <v>41320</v>
       </c>
     </row>
     <row r="248">
@@ -3127,7 +3127,7 @@
         <v>FID. MAROLIO CARACOL 500 Grs</v>
       </c>
       <c r="C248" t="str">
-        <v/>
+        <v>41300</v>
       </c>
     </row>
     <row r="249">
@@ -3138,7 +3138,7 @@
         <v>FID. MAROLIO CELENTANO 500 Grs</v>
       </c>
       <c r="C249" t="str">
-        <v/>
+        <v>41301</v>
       </c>
     </row>
     <row r="250">
@@ -3149,7 +3149,7 @@
         <v>FID. MAROLIO CODITO 500 Grs</v>
       </c>
       <c r="C250" t="str">
-        <v/>
+        <v>41374</v>
       </c>
     </row>
     <row r="251">
@@ -3160,7 +3160,7 @@
         <v>FID. MAROLIO CODOS 500 Grs</v>
       </c>
       <c r="C251" t="str">
-        <v/>
+        <v>41303</v>
       </c>
     </row>
     <row r="252">
@@ -3171,7 +3171,7 @@
         <v>FID. MAROLIO MOSTACHOL 500 Grs</v>
       </c>
       <c r="C252" t="str">
-        <v/>
+        <v>41307</v>
       </c>
     </row>
     <row r="253">
@@ -3182,7 +3182,7 @@
         <v>FID. MAROLIO RIGATTI 500 Grs</v>
       </c>
       <c r="C253" t="str">
-        <v/>
+        <v>41308</v>
       </c>
     </row>
     <row r="254">
@@ -3193,7 +3193,7 @@
         <v>FID. MAROLIO TIRABUZON 500 Grs</v>
       </c>
       <c r="C254" t="str">
-        <v/>
+        <v>41311</v>
       </c>
     </row>
     <row r="255">
@@ -3204,7 +3204,7 @@
         <v>FID. MOLTO SPAGHETTI 500 Grs</v>
       </c>
       <c r="C255" t="str">
-        <v/>
+        <v>41313</v>
       </c>
     </row>
     <row r="256">
@@ -3215,7 +3215,7 @@
         <v>FID. MOLTO TALLARIN 500 Grs</v>
       </c>
       <c r="C256" t="str">
-        <v/>
+        <v>41314</v>
       </c>
     </row>
     <row r="257">
@@ -3226,7 +3226,7 @@
         <v>FID. MAROLIO CAB.ANGEL 500 Grs</v>
       </c>
       <c r="C257" t="str">
-        <v/>
+        <v>41320</v>
       </c>
     </row>
     <row r="258">
@@ -3237,7 +3237,7 @@
         <v>FID. MAROLIO DEDALES 500 Grs</v>
       </c>
       <c r="C258" t="str">
-        <v/>
+        <v>41321</v>
       </c>
     </row>
     <row r="259">
@@ -3248,7 +3248,7 @@
         <v>FID. MAROLIO DEDALON 500 Grs</v>
       </c>
       <c r="C259" t="str">
-        <v/>
+        <v>41322</v>
       </c>
     </row>
     <row r="260">
@@ -3259,7 +3259,7 @@
         <v>FID. MAROLIO MOST.LISO 500 Grs</v>
       </c>
       <c r="C260" t="str">
-        <v/>
+        <v>41323</v>
       </c>
     </row>
     <row r="261">
@@ -3270,7 +3270,7 @@
         <v>FID. MAROLIO SPAGHETTI 500 Grs</v>
       </c>
       <c r="C261" t="str">
-        <v/>
+        <v>41325</v>
       </c>
     </row>
     <row r="262">
@@ -3281,7 +3281,7 @@
         <v>FID. MAROLIO TALLARIN 500 Grs</v>
       </c>
       <c r="C262" t="str">
-        <v/>
+        <v>41326</v>
       </c>
     </row>
     <row r="263">
@@ -3292,7 +3292,7 @@
         <v>FID. MAROLIO DEDALITO 500 Grs</v>
       </c>
       <c r="C263" t="str">
-        <v/>
+        <v>41369</v>
       </c>
     </row>
     <row r="264">
@@ -3303,7 +3303,7 @@
         <v>FID. MAROLIO CODITO 500 Grs</v>
       </c>
       <c r="C264" t="str">
-        <v/>
+        <v>41374</v>
       </c>
     </row>
     <row r="265">
@@ -3314,7 +3314,7 @@
         <v>JARDINERA MAROLIO LATA 300 Grs</v>
       </c>
       <c r="C265" t="str">
-        <v/>
+        <v>41377</v>
       </c>
     </row>
     <row r="266">
@@ -3325,7 +3325,7 @@
         <v>JUGO MOCORETA NARANJA 600 CC.</v>
       </c>
       <c r="C266" t="str">
-        <v/>
+        <v>41385</v>
       </c>
     </row>
     <row r="267">
@@ -3336,7 +3336,7 @@
         <v>ALCOHOL QUEMAR BIALCOHOL 500 ml.</v>
       </c>
       <c r="C267" t="str">
-        <v/>
+        <v>41387</v>
       </c>
     </row>
     <row r="268">
@@ -3347,7 +3347,7 @@
         <v>SNACKS ALMADRE REMOLACHA 130 Grs</v>
       </c>
       <c r="C268" t="str">
-        <v/>
+        <v>41392</v>
       </c>
     </row>
     <row r="269">
@@ -3358,7 +3358,7 @@
         <v>JUGO BAGGIO MIX CITRUS 1 Lt.</v>
       </c>
       <c r="C269" t="str">
-        <v/>
+        <v>41396</v>
       </c>
     </row>
     <row r="270">
@@ -3369,7 +3369,7 @@
         <v>JUGO BAGGIO MIX CITRUS 1.5 Lt.</v>
       </c>
       <c r="C270" t="str">
-        <v/>
+        <v>41397</v>
       </c>
     </row>
     <row r="271">
@@ -3380,7 +3380,7 @@
         <v>GALLETITA CELOSAS TRADICIONAL 350 Grs</v>
       </c>
       <c r="C271" t="str">
-        <v/>
+        <v>41432</v>
       </c>
     </row>
     <row r="272">
@@ -3391,7 +3391,7 @@
         <v>BOCADITOS GRANIX RELLENO FRUTILLA 180 Grs</v>
       </c>
       <c r="C272" t="str">
-        <v/>
+        <v>41435</v>
       </c>
     </row>
     <row r="273">
@@ -3402,7 +3402,7 @@
         <v>NATURITOS GRANIX FRUTOS ROJOS 90 Grs</v>
       </c>
       <c r="C273" t="str">
-        <v/>
+        <v>41437</v>
       </c>
     </row>
     <row r="274">
@@ -3413,7 +3413,7 @@
         <v>ACEITUNA CEBILA 100 Grs</v>
       </c>
       <c r="C274" t="str">
-        <v/>
+        <v>41452</v>
       </c>
     </row>
     <row r="275">
@@ -3424,7 +3424,7 @@
         <v>PEPAS TRIO 320 Grs</v>
       </c>
       <c r="C275" t="str">
-        <v/>
+        <v>41479</v>
       </c>
     </row>
     <row r="276">
@@ -3435,7 +3435,7 @@
         <v>EDULCORANTE CA�UELAS Clasico 100 Un.</v>
       </c>
       <c r="C276" t="str">
-        <v/>
+        <v>41492</v>
       </c>
     </row>
     <row r="277">
@@ -3446,7 +3446,7 @@
         <v>ALCOHOL ET. ALCOPROTEC 96% 500 CC.</v>
       </c>
       <c r="C277" t="str">
-        <v/>
+        <v>41496</v>
       </c>
     </row>
     <row r="278">
@@ -3457,7 +3457,7 @@
         <v>ALCOHOL ET. ALCOPROTEC 96% 1 Lt.</v>
       </c>
       <c r="C278" t="str">
-        <v/>
+        <v>41497</v>
       </c>
     </row>
     <row r="279">
@@ -3468,7 +3468,7 @@
         <v>AZUCAR LEDESMA RUBIA 900 Un.</v>
       </c>
       <c r="C279" t="str">
-        <v/>
+        <v>41499</v>
       </c>
     </row>
     <row r="280">
@@ -3479,7 +3479,7 @@
         <v>MERM. MAROLIO CIRUELA 454 Grs</v>
       </c>
       <c r="C280" t="str">
-        <v/>
+        <v>41900</v>
       </c>
     </row>
     <row r="281">
@@ -3490,7 +3490,7 @@
         <v>MERM. MAROLIO DAMASCO 454 Grs</v>
       </c>
       <c r="C281" t="str">
-        <v/>
+        <v>41901</v>
       </c>
     </row>
     <row r="282">
@@ -3501,7 +3501,7 @@
         <v>MERM. MAROLIO DURAZNO 454 Grs</v>
       </c>
       <c r="C282" t="str">
-        <v/>
+        <v>41902</v>
       </c>
     </row>
     <row r="283">
@@ -3512,7 +3512,7 @@
         <v>ENCENDEDOR CANDELA Un.</v>
       </c>
       <c r="C283" t="str">
-        <v/>
+        <v>41915</v>
       </c>
     </row>
     <row r="284">
@@ -3523,7 +3523,7 @@
         <v>ACELGA LA BANDA LATA 800 Grs</v>
       </c>
       <c r="C284" t="str">
-        <v/>
+        <v>42000</v>
       </c>
     </row>
     <row r="285">
@@ -3534,7 +3534,7 @@
         <v>ARVEJA LA BANDA LATA 800 Grs</v>
       </c>
       <c r="C285" t="str">
-        <v/>
+        <v>42001</v>
       </c>
     </row>
     <row r="286">
@@ -3545,7 +3545,7 @@
         <v>ESPINACA LA BANDA LATA 800 Grs</v>
       </c>
       <c r="C286" t="str">
-        <v/>
+        <v>42002</v>
       </c>
     </row>
     <row r="287">
@@ -3556,7 +3556,7 @@
         <v>CHOCLO GR.AMAR LA BANDA LATA 810 Grs</v>
       </c>
       <c r="C287" t="str">
-        <v/>
+        <v>42003</v>
       </c>
     </row>
     <row r="288">
@@ -3567,7 +3567,7 @@
         <v>TOMATE ENTERO LA BANDA LATA 8 Kgs</v>
       </c>
       <c r="C288" t="str">
-        <v/>
+        <v>42004</v>
       </c>
     </row>
     <row r="289">
@@ -3578,7 +3578,7 @@
         <v>ACEITUNA CASTELL BALDE 5 Kgs</v>
       </c>
       <c r="C289" t="str">
-        <v/>
+        <v>42010</v>
       </c>
     </row>
     <row r="290">
@@ -3589,7 +3589,7 @@
         <v>SAL GRUESA DOS ESTRELLAS 1 Kgs</v>
       </c>
       <c r="C290" t="str">
-        <v/>
+        <v>50123</v>
       </c>
     </row>
     <row r="291">
@@ -3600,7 +3600,7 @@
         <v>SAL FINA GENSER SALERO 90 Grs</v>
       </c>
       <c r="C291" t="str">
-        <v/>
+        <v>50181</v>
       </c>
     </row>
     <row r="292">
@@ -3611,7 +3611,7 @@
         <v>SAL FINA CELUSAL SOBRES 1000 Un.</v>
       </c>
       <c r="C292" t="str">
-        <v/>
+        <v>50199</v>
       </c>
     </row>
     <row r="293">
@@ -3622,7 +3622,7 @@
         <v>T.FEMENINA CALIPSO C/ALAS C/DEO 8 Un.</v>
       </c>
       <c r="C293" t="str">
-        <v/>
+        <v>50248</v>
       </c>
     </row>
     <row r="294">
@@ -3633,7 +3633,7 @@
         <v>T.FEMENINA CALIPSO S/ALAS S/DEO 8 Un.</v>
       </c>
       <c r="C294" t="str">
-        <v/>
+        <v>50249</v>
       </c>
     </row>
     <row r="295">
@@ -3644,7 +3644,7 @@
         <v>T.FEMENINA CALIPSO S/ALAS C/DEO 8 Un.</v>
       </c>
       <c r="C295" t="str">
-        <v/>
+        <v>50250</v>
       </c>
     </row>
     <row r="296">
@@ -3655,7 +3655,7 @@
         <v>PROTECTOR CALIPSO COLA LESS 20 Un.</v>
       </c>
       <c r="C296" t="str">
-        <v/>
+        <v>50254</v>
       </c>
     </row>
     <row r="297">
@@ -3666,7 +3666,7 @@
         <v>TAMPONES NOSOTRAS REGULAR 8 Un.</v>
       </c>
       <c r="C297" t="str">
-        <v/>
+        <v>50267</v>
       </c>
     </row>
     <row r="298">
@@ -3677,7 +3677,7 @@
         <v>TAMPONES NOSOTRAS SUPER 8 Un.</v>
       </c>
       <c r="C298" t="str">
-        <v/>
+        <v>50268</v>
       </c>
     </row>
     <row r="299">
@@ -3688,7 +3688,7 @@
         <v>DISCOS DONCELLA ALGODON 80 Un.</v>
       </c>
       <c r="C299" t="str">
-        <v/>
+        <v>50430</v>
       </c>
     </row>
     <row r="300">
@@ -3699,7 +3699,7 @@
         <v>PA�UELOS ELITE 10 Un.</v>
       </c>
       <c r="C300" t="str">
-        <v/>
+        <v>51020</v>
       </c>
     </row>
     <row r="301">
@@ -3710,7 +3710,7 @@
         <v>P.HIGIENICO HIGIENOL DH PLUS 30Mx4 Un.</v>
       </c>
       <c r="C301" t="str">
-        <v/>
+        <v>51030</v>
       </c>
     </row>
     <row r="302">
@@ -3721,7 +3721,7 @@
         <v>P.HIGIENICO HIGIENOL HS 30Mx4 Un.</v>
       </c>
       <c r="C302" t="str">
-        <v/>
+        <v>51031</v>
       </c>
     </row>
     <row r="303">
@@ -3732,7 +3732,7 @@
         <v>SERVILLETA SUSSEX 30x30 140 Un.</v>
       </c>
       <c r="C303" t="str">
-        <v/>
+        <v>51043</v>
       </c>
     </row>
     <row r="304">
@@ -3743,7 +3743,7 @@
         <v>PA�AL BABYSEC PREMIUM G 9 Un.</v>
       </c>
       <c r="C304" t="str">
-        <v/>
+        <v>51050</v>
       </c>
     </row>
     <row r="305">
@@ -3754,7 +3754,7 @@
         <v>PA�AL BABYSEC PREMIUM M 10 Un.</v>
       </c>
       <c r="C305" t="str">
-        <v/>
+        <v>51051</v>
       </c>
     </row>
     <row r="306">
@@ -3765,7 +3765,7 @@
         <v>PA�AL BABYSEC PREMIUM P 12 Un.</v>
       </c>
       <c r="C306" t="str">
-        <v/>
+        <v>51052</v>
       </c>
     </row>
     <row r="307">
@@ -3776,7 +3776,7 @@
         <v>PA�AL BABYSEC PREMIUM XG 8 Un.</v>
       </c>
       <c r="C307" t="str">
-        <v/>
+        <v>51053</v>
       </c>
     </row>
     <row r="308">
@@ -3787,7 +3787,7 @@
         <v>PA�AL BABYSEC PREMIUM XXG 8 Un.</v>
       </c>
       <c r="C308" t="str">
-        <v/>
+        <v>51054</v>
       </c>
     </row>
     <row r="309">
@@ -3798,7 +3798,7 @@
         <v>T.FEMENINA LADYSOFT NORMAL SECA 8 Un.</v>
       </c>
       <c r="C309" t="str">
-        <v/>
+        <v>51083</v>
       </c>
     </row>
     <row r="310">
@@ -3809,7 +3809,7 @@
         <v>VINO SEXY FISH Malbec 750 CC.</v>
       </c>
       <c r="C310" t="str">
-        <v/>
+        <v>60001</v>
       </c>
     </row>
     <row r="311">
@@ -3820,7 +3820,7 @@
         <v>VINO COSECHA TARDIA BLANCO 750 CC.</v>
       </c>
       <c r="C311" t="str">
-        <v/>
+        <v>60022</v>
       </c>
     </row>
     <row r="312">
@@ -3831,7 +3831,7 @@
         <v>VINO VASCO VIEJO BLANCO 750 CC.</v>
       </c>
       <c r="C312" t="str">
-        <v/>
+        <v>60080</v>
       </c>
     </row>
     <row r="313">
@@ -3842,7 +3842,7 @@
         <v>VINO VASCO VIEJO TINTO 750 CC.</v>
       </c>
       <c r="C313" t="str">
-        <v/>
+        <v>60081</v>
       </c>
     </row>
     <row r="314">
@@ -3853,7 +3853,7 @@
         <v>VINO SUC. ABEL M.T. BLANCO 700 CC.</v>
       </c>
       <c r="C314" t="str">
-        <v/>
+        <v>60102</v>
       </c>
     </row>
     <row r="315">
@@ -3864,7 +3864,7 @@
         <v>VINO SUC. ABEL M.T. TINTO 700 CC.</v>
       </c>
       <c r="C315" t="str">
-        <v/>
+        <v>60103</v>
       </c>
     </row>
     <row r="316">
@@ -3875,7 +3875,7 @@
         <v>VINO KILLKA MALBEC 750 CC.</v>
       </c>
       <c r="C316" t="str">
-        <v/>
+        <v>60152</v>
       </c>
     </row>
     <row r="317">
@@ -3886,7 +3886,7 @@
         <v>VINO KILLKA CABERNET 750 CC.</v>
       </c>
       <c r="C317" t="str">
-        <v/>
+        <v>60153</v>
       </c>
     </row>
     <row r="318">
@@ -3897,7 +3897,7 @@
         <v>VINO HORMIGA NEGRA CABERNET 750 CC.</v>
       </c>
       <c r="C318" t="str">
-        <v/>
+        <v>60182</v>
       </c>
     </row>
     <row r="319">
@@ -3908,7 +3908,7 @@
         <v>VINO HORMIGA NEGRA MALBEC 750 CC.</v>
       </c>
       <c r="C319" t="str">
-        <v/>
+        <v>60183</v>
       </c>
     </row>
     <row r="320">
@@ -3919,7 +3919,7 @@
         <v>VINO ALAMOS CHARDONNAY 750 CC.</v>
       </c>
       <c r="C320" t="str">
-        <v/>
+        <v>60325</v>
       </c>
     </row>
     <row r="321">
@@ -3930,7 +3930,7 @@
         <v>VINO ALAMOS CABERNET 750 CC.</v>
       </c>
       <c r="C321" t="str">
-        <v/>
+        <v>60326</v>
       </c>
     </row>
     <row r="322">
@@ -3941,7 +3941,7 @@
         <v>VINO ALAMOS DCE.NATURAL 750 CC.</v>
       </c>
       <c r="C322" t="str">
-        <v/>
+        <v>60328</v>
       </c>
     </row>
     <row r="323">
@@ -3952,7 +3952,7 @@
         <v>VINO ALAMOS MALBEC 750 CC.</v>
       </c>
       <c r="C323" t="str">
-        <v/>
+        <v>60329</v>
       </c>
     </row>
     <row r="324">
@@ -3963,7 +3963,7 @@
         <v>VINO S.FELICIEN CABERNET 750 CC.</v>
       </c>
       <c r="C324" t="str">
-        <v/>
+        <v>60330</v>
       </c>
     </row>
     <row r="325">
@@ -3974,7 +3974,7 @@
         <v>VINO S.FELICIEN CAB/MERLOT 750 CC.</v>
       </c>
       <c r="C325" t="str">
-        <v/>
+        <v>60331</v>
       </c>
     </row>
     <row r="326">
@@ -3985,7 +3985,7 @@
         <v>VINO S.FELICIEN CHARDONNAY 750 CC.</v>
       </c>
       <c r="C326" t="str">
-        <v/>
+        <v>60332</v>
       </c>
     </row>
     <row r="327">
@@ -3996,7 +3996,7 @@
         <v>VINO S.FELICIEN MALBEC 750 CC.</v>
       </c>
       <c r="C327" t="str">
-        <v/>
+        <v>60364</v>
       </c>
     </row>
     <row r="328">
@@ -4007,7 +4007,7 @@
         <v>VINO TORO TINTO T/B 1 Lt.</v>
       </c>
       <c r="C328" t="str">
-        <v/>
+        <v>60370</v>
       </c>
     </row>
     <row r="329">
@@ -4018,7 +4018,7 @@
         <v>VINO ANGELICA ZAPATA MALBEC 750 CC.</v>
       </c>
       <c r="C329" t="str">
-        <v/>
+        <v>60381</v>
       </c>
     </row>
     <row r="330">
@@ -4029,7 +4029,7 @@
         <v>VINO S HUBERTO CABERNET 750 CC.</v>
       </c>
       <c r="C330" t="str">
-        <v/>
+        <v>60432</v>
       </c>
     </row>
     <row r="331">
@@ -4040,7 +4040,7 @@
         <v>VINO S HUBERTO MALBEC 750 CC.</v>
       </c>
       <c r="C331" t="str">
-        <v/>
+        <v>60433</v>
       </c>
     </row>
     <row r="332">
@@ -4051,7 +4051,7 @@
         <v>VINO TRUMPETER CAB.FRANC 750 CC.</v>
       </c>
       <c r="C332" t="str">
-        <v/>
+        <v>60459</v>
       </c>
     </row>
     <row r="333">
@@ -4062,7 +4062,7 @@
         <v>VINO TRUMPETER CHARDONNAY 750 CC.</v>
       </c>
       <c r="C333" t="str">
-        <v/>
+        <v>60460</v>
       </c>
     </row>
     <row r="334">
@@ -4073,7 +4073,7 @@
         <v>VINO TRUMPETER CABERNET 750 CC.</v>
       </c>
       <c r="C334" t="str">
-        <v/>
+        <v>60461</v>
       </c>
     </row>
     <row r="335">
@@ -4084,7 +4084,7 @@
         <v>VINO TRUMPETER MALBEC 750 CC.</v>
       </c>
       <c r="C335" t="str">
-        <v/>
+        <v>60462</v>
       </c>
     </row>
     <row r="336">
@@ -4095,7 +4095,7 @@
         <v>VINO TRUMPETER MERLOT 750 CC.</v>
       </c>
       <c r="C336" t="str">
-        <v/>
+        <v>60463</v>
       </c>
     </row>
     <row r="337">
@@ -4106,7 +4106,7 @@
         <v>VINO TRUMPETER SYRAH 750 CC.</v>
       </c>
       <c r="C337" t="str">
-        <v/>
+        <v>60464</v>
       </c>
     </row>
     <row r="338">
@@ -4117,7 +4117,7 @@
         <v>VINO MIL ROSAS ROSADO 750 CC.</v>
       </c>
       <c r="C338" t="str">
-        <v/>
+        <v>60477</v>
       </c>
     </row>
     <row r="339">
@@ -4128,7 +4128,7 @@
         <v>VINO ALAMOS RED BLEND 750 CC.</v>
       </c>
       <c r="C339" t="str">
-        <v/>
+        <v>60524</v>
       </c>
     </row>
     <row r="340">
@@ -4139,7 +4139,7 @@
         <v>VINO S.FELICIEN SYRAH 750 CC.</v>
       </c>
       <c r="C340" t="str">
-        <v/>
+        <v>60577</v>
       </c>
     </row>
     <row r="341">
@@ -4150,7 +4150,7 @@
         <v>VINO SUC. ABEL M.T. ABOCADO 700 CC.</v>
       </c>
       <c r="C341" t="str">
-        <v/>
+        <v>60578</v>
       </c>
     </row>
     <row r="342">
@@ -4161,7 +4161,7 @@
         <v>VINO ETCHART TORRONTES 750 CC.</v>
       </c>
       <c r="C342" t="str">
-        <v/>
+        <v>60790</v>
       </c>
     </row>
     <row r="343">
@@ -4172,7 +4172,7 @@
         <v>VINO ALAMBRADO MALBEC 750 CC.</v>
       </c>
       <c r="C343" t="str">
-        <v/>
+        <v>60812</v>
       </c>
     </row>
     <row r="344">
@@ -4183,7 +4183,7 @@
         <v>VINO ALAMBRADO CABERNET 750 CC.</v>
       </c>
       <c r="C344" t="str">
-        <v/>
+        <v>60813</v>
       </c>
     </row>
     <row r="345">
@@ -4194,7 +4194,7 @@
         <v>VINO ESC.GASCON CAB.FRANC 750 CC.</v>
       </c>
       <c r="C345" t="str">
-        <v/>
+        <v>60829</v>
       </c>
     </row>
     <row r="346">
@@ -4205,7 +4205,7 @@
         <v>VINO PECADO COS.TARDIA 750 CC.</v>
       </c>
       <c r="C346" t="str">
-        <v/>
+        <v>60844</v>
       </c>
     </row>
     <row r="347">
@@ -4216,7 +4216,7 @@
         <v>VINO LOPEZ CABERNET 750 CC.</v>
       </c>
       <c r="C347" t="str">
-        <v/>
+        <v>60865</v>
       </c>
     </row>
     <row r="348">
@@ -4227,7 +4227,7 @@
         <v>VINO COSECHA TARDIA TINTO 750 CC.</v>
       </c>
       <c r="C348" t="str">
-        <v/>
+        <v>60914</v>
       </c>
     </row>
     <row r="349">
@@ -4238,7 +4238,7 @@
         <v>VINO EMILIA MALBEC 750 CC.</v>
       </c>
       <c r="C349" t="str">
-        <v/>
+        <v>60918</v>
       </c>
     </row>
     <row r="350">
@@ -4249,7 +4249,7 @@
         <v>VINO ESC.GASCON CABERNET 750 CC.</v>
       </c>
       <c r="C350" t="str">
-        <v/>
+        <v>60925</v>
       </c>
     </row>
     <row r="351">
@@ -4260,7 +4260,7 @@
         <v>VINO COSECHA TARDIA ROSADO 750 CC.</v>
       </c>
       <c r="C351" t="str">
-        <v/>
+        <v>60927</v>
       </c>
     </row>
     <row r="352">
@@ -4271,7 +4271,7 @@
         <v>VINO TORO TINTO 700 CC.</v>
       </c>
       <c r="C352" t="str">
-        <v/>
+        <v>60956</v>
       </c>
     </row>
     <row r="353">
@@ -4282,7 +4282,7 @@
         <v>VINO E.MENDOZA CAB/MALBEC 750 CC.</v>
       </c>
       <c r="C353" t="str">
-        <v/>
+        <v>60968</v>
       </c>
     </row>
     <row r="354">
@@ -4293,7 +4293,7 @@
         <v>VINO E.MENDOZA MER/MALBEC 750 CC.</v>
       </c>
       <c r="C354" t="str">
-        <v/>
+        <v>60969</v>
       </c>
     </row>
     <row r="355">
@@ -4304,7 +4304,7 @@
         <v>VINO E.MENDOZA CHAR/CHENNIN 750 CC.</v>
       </c>
       <c r="C355" t="str">
-        <v/>
+        <v>60970</v>
       </c>
     </row>
     <row r="356">
@@ -4315,7 +4315,7 @@
         <v>VINO CANCILLER ED.ESPEC 1.125 CC.</v>
       </c>
       <c r="C356" t="str">
-        <v/>
+        <v>60972</v>
       </c>
     </row>
     <row r="357">
@@ -4326,7 +4326,7 @@
         <v>VINO DILEMA BCO.DULCE 750 CC.</v>
       </c>
       <c r="C357" t="str">
-        <v/>
+        <v>60973</v>
       </c>
     </row>
     <row r="358">
@@ -4337,7 +4337,7 @@
         <v>VINO DILEMA ROSADO DCE 750 CC.</v>
       </c>
       <c r="C358" t="str">
-        <v/>
+        <v>60974</v>
       </c>
     </row>
     <row r="359">
@@ -4348,7 +4348,7 @@
         <v>VINO ESC.GASCON MALBEC 750 CC.</v>
       </c>
       <c r="C359" t="str">
-        <v/>
+        <v>61003</v>
       </c>
     </row>
     <row r="360">
@@ -4359,7 +4359,7 @@
         <v>VINO E.MENDOZA CHENIN DCE 750 CC.</v>
       </c>
       <c r="C360" t="str">
-        <v/>
+        <v>61018</v>
       </c>
     </row>
     <row r="361">
@@ -4370,7 +4370,7 @@
         <v>VINO UXMAL ALTO MALBEC 750 CC.</v>
       </c>
       <c r="C361" t="str">
-        <v/>
+        <v>61036</v>
       </c>
     </row>
     <row r="362">
@@ -4381,7 +4381,7 @@
         <v>VINO CALLIA MALBEC 750 CC.</v>
       </c>
       <c r="C362" t="str">
-        <v/>
+        <v>61048</v>
       </c>
     </row>
     <row r="363">
@@ -4392,7 +4392,7 @@
         <v>VINO CALLIA CABERNET 750 CC.</v>
       </c>
       <c r="C363" t="str">
-        <v/>
+        <v>61051</v>
       </c>
     </row>
     <row r="364">
@@ -4403,7 +4403,7 @@
         <v>VINO C.MADERO CABERNET 750 CC.</v>
       </c>
       <c r="C364" t="str">
-        <v/>
+        <v>61061</v>
       </c>
     </row>
     <row r="365">
@@ -4414,7 +4414,7 @@
         <v>VINO C.MADERO MALBEC 750 CC.</v>
       </c>
       <c r="C365" t="str">
-        <v/>
+        <v>61062</v>
       </c>
     </row>
     <row r="366">

</xml_diff>